<commit_message>
Optimization, arguments, timer update
</commit_message>
<xml_diff>
--- a/examples/runtimes.xlsx
+++ b/examples/runtimes.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nck\repos\nmacom\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A62CEA-7007-4E02-A546-05671F61B842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D173CE7E-3E72-4026-B90F-111B05320832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{6DD579A3-6919-4BFE-930E-E1B31D758E9F}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{6DD579A3-6919-4BFE-930E-E1B31D758E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -40,42 +40,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Noah Cohen Kalafut</author>
-  </authors>
-  <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0CCAFBBA-52DA-44FE-955E-350181D48D5D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Noah Cohen Kalafut:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Default 2000 iterations on all matrices</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
   <si>
     <t>Cells</t>
   </si>
@@ -146,39 +112,32 @@
     <t>Two Step Total</t>
   </si>
   <si>
-    <t>(Multiple Items)</t>
-  </si>
-  <si>
     <t>Solution collapses, but should be equivalent in runtime</t>
   </si>
   <si>
-    <t>500, (Small Matrix 1000, Large 2000)</t>
+    <t>Matrix Sizes</t>
+  </si>
+  <si>
+    <t>1000 Small, 2000 Large</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>After additional optimizations to grad calculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1204,7 +1163,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Visualization!$B$5:$B$7</c:f>
+              <c:f>Visualization!$B$6:$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1239,7 +1198,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Visualization!$A$8:$A$13</c:f>
+              <c:f>Visualization!$A$9:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1262,7 +1221,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Visualization!$B$8:$B$13</c:f>
+              <c:f>Visualization!$B$9:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1284,7 +1243,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Visualization!$D$5:$D$7</c:f>
+              <c:f>Visualization!$D$6:$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1319,7 +1278,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Visualization!$A$8:$A$13</c:f>
+              <c:f>Visualization!$A$9:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1342,7 +1301,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Visualization!$D$8:$D$13</c:f>
+              <c:f>Visualization!$D$9:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1364,7 +1323,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Visualization!$E$5:$E$7</c:f>
+              <c:f>Visualization!$E$6:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1399,7 +1358,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Visualization!$A$8:$A$13</c:f>
+              <c:f>Visualization!$A$9:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1422,7 +1381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Visualization!$E$8:$E$13</c:f>
+              <c:f>Visualization!$E$9:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1453,7 +1412,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Visualization!$G$5:$G$7</c:f>
+              <c:f>Visualization!$G$6:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1488,7 +1447,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Visualization!$A$8:$A$13</c:f>
+              <c:f>Visualization!$A$9:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1511,7 +1470,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Visualization!$G$8:$G$13</c:f>
+              <c:f>Visualization!$G$9:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2452,11 +2411,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Noah Cohen Kalafut" refreshedDate="44489.598581134262" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="16" xr:uid="{EF2E8102-1807-46C2-A695-492AF07769EF}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Noah Cohen Kalafut" refreshedDate="44494.912168171293" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="16" xr:uid="{EF2E8102-1807-46C2-A695-492AF07769EF}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I17" sheet="Data"/>
+    <worksheetSource ref="A1:J17" sheet="Data"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="10">
     <cacheField name="Cells" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="500" maxValue="22463" count="6">
         <n v="500"/>
@@ -2482,13 +2441,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Time (s)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="8" maxValue="2776" count="16">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="2776" count="16">
         <n v="34"/>
         <n v="25"/>
         <n v="16"/>
         <n v="125"/>
         <n v="109"/>
-        <m/>
+        <n v="980"/>
         <n v="119"/>
         <n v="120"/>
         <n v="8"/>
@@ -2509,6 +2468,12 @@
         <s v="None"/>
         <s v="Gradient Reduction"/>
         <s v="Two Step"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Matrix Sizes" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="2000" maxValue="2000" count="2">
+        <n v="2000"/>
+        <s v="1000 Small, 2000 Large"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Arguments" numFmtId="0">
@@ -2541,6 +2506,7 @@
     <x v="0"/>
     <s v="Euclidean"/>
     <x v="0"/>
+    <x v="0"/>
     <m/>
     <x v="0"/>
     <m/>
@@ -2552,6 +2518,7 @@
     <x v="1"/>
     <s v="Euclidean"/>
     <x v="1"/>
+    <x v="0"/>
     <s v="100, .99"/>
     <x v="0"/>
     <m/>
@@ -2563,6 +2530,7 @@
     <x v="2"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="10"/>
     <x v="0"/>
     <m/>
@@ -2574,6 +2542,7 @@
     <x v="3"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="10"/>
     <x v="0"/>
     <m/>
@@ -2585,6 +2554,7 @@
     <x v="4"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="50"/>
     <x v="0"/>
     <m/>
@@ -2596,9 +2566,10 @@
     <x v="5"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="1"/>
     <n v="500"/>
     <x v="0"/>
-    <s v="Large F collapse; Kernel crash"/>
+    <s v="Solution collapses, but should be equivalent in runtime"/>
   </r>
   <r>
     <x v="1"/>
@@ -2606,6 +2577,7 @@
     <x v="1"/>
     <x v="6"/>
     <s v="Euclidean"/>
+    <x v="0"/>
     <x v="0"/>
     <m/>
     <x v="1"/>
@@ -2618,6 +2590,7 @@
     <x v="7"/>
     <s v="Euclidean"/>
     <x v="0"/>
+    <x v="0"/>
     <m/>
     <x v="1"/>
     <m/>
@@ -2628,6 +2601,7 @@
     <x v="0"/>
     <x v="8"/>
     <s v="Euclidean"/>
+    <x v="0"/>
     <x v="0"/>
     <m/>
     <x v="1"/>
@@ -2640,6 +2614,7 @@
     <x v="9"/>
     <s v="Euclidean"/>
     <x v="0"/>
+    <x v="0"/>
     <m/>
     <x v="1"/>
     <m/>
@@ -2651,6 +2626,7 @@
     <x v="10"/>
     <s v="Euclidean"/>
     <x v="0"/>
+    <x v="0"/>
     <m/>
     <x v="1"/>
     <m/>
@@ -2662,6 +2638,7 @@
     <x v="11"/>
     <s v="Euclidean"/>
     <x v="0"/>
+    <x v="0"/>
     <m/>
     <x v="1"/>
     <m/>
@@ -2673,6 +2650,7 @@
     <x v="12"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="20"/>
     <x v="0"/>
     <m/>
@@ -2684,6 +2662,7 @@
     <x v="13"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="50"/>
     <x v="0"/>
     <m/>
@@ -2695,6 +2674,7 @@
     <x v="14"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="200"/>
     <x v="0"/>
     <m/>
@@ -2706,6 +2686,7 @@
     <x v="15"/>
     <s v="Euclidean"/>
     <x v="2"/>
+    <x v="0"/>
     <n v="400"/>
     <x v="0"/>
     <m/>
@@ -2715,8 +2696,8 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E365D83-FC29-415B-96E0-1FDBC73826DC}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A5:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="9">
+  <location ref="A6:I14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item x="0"/>
@@ -2761,7 +2742,7 @@
         <item x="14"/>
         <item x="11"/>
         <item x="15"/>
-        <item h="1" x="5"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2771,6 +2752,13 @@
         <item x="1"/>
         <item x="0"/>
         <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2809,7 +2797,7 @@
   </rowItems>
   <colFields count="2">
     <field x="5"/>
-    <field x="7"/>
+    <field x="8"/>
   </colFields>
   <colItems count="8">
     <i>
@@ -2840,10 +2828,11 @@
       <x/>
     </i>
   </colItems>
-  <pageFields count="3">
+  <pageFields count="4">
     <pageField fld="3" hier="-1"/>
     <pageField fld="1" hier="-1"/>
     <pageField fld="2" hier="-1"/>
+    <pageField fld="6" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Min of Time (s)" fld="3" subtotal="min" baseField="0" baseItem="0"/>
@@ -2855,7 +2844,7 @@
           <reference field="5" count="1" selected="0">
             <x v="0"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2867,7 +2856,7 @@
           <reference field="5" count="1" selected="0">
             <x v="1"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2879,7 +2868,7 @@
           <reference field="5" count="1" selected="0">
             <x v="1"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
@@ -2891,7 +2880,7 @@
           <reference field="5" count="1" selected="0">
             <x v="2"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2906,7 +2895,7 @@
           <reference field="5" count="1" selected="0">
             <x v="0"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2921,7 +2910,7 @@
           <reference field="5" count="1" selected="0">
             <x v="1"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2936,7 +2925,7 @@
           <reference field="5" count="1" selected="0">
             <x v="1"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
@@ -2951,7 +2940,7 @@
           <reference field="5" count="1" selected="0">
             <x v="2"/>
           </reference>
-          <reference field="7" count="1" selected="0">
+          <reference field="8" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -3267,10 +3256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F7F1FA-5AF1-497D-971C-01C8C2691D02}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3313,7 +3302,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3332,197 +3321,205 @@
         <v>116490</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>500</v>
-      </c>
-      <c r="B8" s="2">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2">
-        <v>16</v>
-      </c>
-      <c r="H8" s="2">
-        <v>16</v>
-      </c>
-      <c r="I8" s="2">
-        <v>8</v>
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>1000</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+        <v>500</v>
+      </c>
+      <c r="B9" s="2">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>34</v>
+      </c>
       <c r="E9" s="2">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H9" s="2">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2">
-        <v>158</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2">
-        <v>158</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="H10" s="2">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2">
-        <v>97</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2">
-        <v>852</v>
+        <v>158</v>
       </c>
       <c r="F11" s="2">
-        <v>852</v>
+        <v>158</v>
       </c>
       <c r="G11" s="2">
-        <v>433</v>
+        <v>97</v>
       </c>
       <c r="H11" s="2">
-        <v>433</v>
+        <v>97</v>
       </c>
       <c r="I11" s="2">
-        <v>433</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="2">
+        <v>852</v>
+      </c>
+      <c r="F12" s="2">
+        <v>852</v>
+      </c>
       <c r="G12" s="2">
-        <v>2776</v>
+        <v>433</v>
       </c>
       <c r="H12" s="2">
-        <v>2776</v>
+        <v>433</v>
       </c>
       <c r="I12" s="2">
-        <v>2776</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="4">
+        <v>8000</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <v>2776</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2776</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>25</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C14" s="2">
         <v>25</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>34</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <v>8</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <v>8</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <v>16</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <v>16</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I14" s="2">
         <v>8</v>
       </c>
     </row>
@@ -3533,11 +3530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5904BA9B-35FB-46AE-840C-47696E629D27}">
-  <dimension ref="A1:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5904BA9B-35FB-46AE-840C-47696E629D27}">
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,13 +3544,13 @@
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="49.28515625" customWidth="1"/>
+    <col min="6" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3573,16 +3570,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>500</v>
       </c>
@@ -3601,13 +3601,16 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>500</v>
       </c>
@@ -3626,15 +3629,18 @@
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>500</v>
       </c>
@@ -3654,14 +3660,17 @@
         <v>14</v>
       </c>
       <c r="G4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2000</v>
       </c>
@@ -3681,14 +3690,17 @@
         <v>14</v>
       </c>
       <c r="G5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H5" s="1">
         <v>10</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2000</v>
       </c>
@@ -3708,14 +3720,17 @@
         <v>14</v>
       </c>
       <c r="G6" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="1">
         <v>50</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>22463</v>
       </c>
@@ -3737,14 +3752,17 @@
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="1">
+        <v>500</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
+      <c r="J7" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2000</v>
       </c>
@@ -3763,13 +3781,16 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2000</v>
       </c>
@@ -3788,13 +3809,16 @@
       <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
+      <c r="G9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>500</v>
       </c>
@@ -3813,13 +3837,16 @@
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1000</v>
       </c>
@@ -3838,13 +3865,16 @@
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2000</v>
       </c>
@@ -3863,13 +3893,16 @@
       <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
+      <c r="G12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4000</v>
       </c>
@@ -3888,13 +3921,16 @@
       <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
+      <c r="G13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1000</v>
       </c>
@@ -3914,14 +3950,17 @@
         <v>14</v>
       </c>
       <c r="G14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H14" s="1">
         <v>20</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2000</v>
       </c>
@@ -3941,14 +3980,17 @@
         <v>14</v>
       </c>
       <c r="G15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H15" s="1">
         <v>50</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4000</v>
       </c>
@@ -3968,14 +4010,17 @@
         <v>14</v>
       </c>
       <c r="G16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H16" s="1">
         <v>200</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8000</v>
       </c>
@@ -3995,17 +4040,51 @@
         <v>14</v>
       </c>
       <c r="G17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H17" s="1">
         <v>400</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>22463</v>
+      </c>
+      <c r="B18" s="1">
+        <v>13431</v>
+      </c>
+      <c r="C18" s="1">
+        <v>116490</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1494</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17" xr:uid="{5904BA9B-35FB-46AE-840C-47696E629D27}"/>
+  <autoFilter ref="A1:I17" xr:uid="{5904BA9B-35FB-46AE-840C-47696E629D27}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>